<commit_message>
Add table comment function to mysql exporter
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -14,15 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>third_sheet</t>
   </si>
   <si>
+    <t>first_sheet</t>
+  </si>
+  <si>
+    <t>second_sheet</t>
+  </si>
+  <si>
+    <t>first sheet</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>second_sheet</t>
+    <t>third sheet</t>
   </si>
   <si>
     <t>test</t>
@@ -64,61 +73,58 @@
     <t>modified_time</t>
   </si>
   <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>modified time</t>
+  </si>
+  <si>
+    <t>modified_user</t>
+  </si>
+  <si>
+    <t>VARCHAR(45)</t>
+  </si>
+  <si>
+    <t>modified user</t>
+  </si>
+  <si>
     <t>first_sheet_id</t>
   </si>
   <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>modified time</t>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>BIT(1)</t>
+  </si>
+  <si>
+    <t>first_column</t>
   </si>
   <si>
     <t>first_sheet.id</t>
   </si>
   <si>
-    <t>modified_user</t>
-  </si>
-  <si>
-    <t>VARCHAR(45)</t>
-  </si>
-  <si>
-    <t>modified user</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>BIT(1)</t>
-  </si>
-  <si>
-    <t>first_column</t>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second_column</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>Fun: NOW()</t>
   </si>
   <si>
     <t>one</t>
   </si>
   <si>
-    <t>second_column</t>
-  </si>
-  <si>
     <t>two</t>
   </si>
   <si>
     <t>third_column</t>
   </si>
   <si>
-    <t>Fun: NOW()</t>
-  </si>
-  <si>
     <t>third</t>
-  </si>
-  <si>
-    <t>first_sheet</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second</t>
   </si>
   <si>
     <t>fourth_sheet</t>
@@ -210,36 +216,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="3"/>
@@ -261,10 +270,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>1</v>
@@ -280,29 +289,29 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="b">
         <v>1</v>
@@ -314,57 +323,61 @@
         <v>-1.0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" ht="11.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>0.0</v>
+      </c>
       <c r="I12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -386,34 +399,34 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
@@ -435,11 +448,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>1</v>
@@ -455,123 +468,127 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="12" ht="11.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>0.0</v>
+      </c>
       <c r="J14" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -593,37 +610,40 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
@@ -645,11 +665,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
@@ -657,49 +677,49 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" ht="11.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -716,39 +736,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>

</xml_diff>

<commit_message>
Add check function of create defintion to general exporter
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -16,24 +16,24 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
+    <t>first_sheet</t>
+  </si>
+  <si>
+    <t>second_sheet</t>
+  </si>
+  <si>
     <t>third_sheet</t>
   </si>
   <si>
-    <t>first_sheet</t>
-  </si>
-  <si>
-    <t>second_sheet</t>
-  </si>
-  <si>
-    <t>first sheet</t>
+    <t>first sheet comment</t>
+  </si>
+  <si>
+    <t>third sheet comment</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>third sheet</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -88,40 +88,40 @@
     <t>modified user</t>
   </si>
   <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>BIT(1)</t>
+  </si>
+  <si>
     <t>first_sheet_id</t>
   </si>
   <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>BIT(1)</t>
+    <t>first_sheet.id</t>
   </si>
   <si>
     <t>first_column</t>
   </si>
   <si>
-    <t>first_sheet.id</t>
-  </si>
-  <si>
     <t>first</t>
   </si>
   <si>
     <t>second_column</t>
   </si>
   <si>
+    <t>one</t>
+  </si>
+  <si>
     <t>second</t>
   </si>
   <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>third_column</t>
+  </si>
+  <si>
     <t>Fun: NOW()</t>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>third_column</t>
   </si>
   <si>
     <t>third</t>
@@ -216,7 +216,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -224,7 +224,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -294,7 +294,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
@@ -323,7 +323,7 @@
         <v>-1.0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
@@ -342,7 +342,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>20</v>
@@ -365,10 +365,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E12" s="1" t="b">
         <v>1</v>
@@ -377,7 +377,7 @@
         <v>0.0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -394,12 +394,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -473,18 +473,18 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
@@ -512,12 +512,12 @@
         <v>6</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -527,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>36</v>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>20</v>
@@ -575,11 +575,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="1" t="b">
         <v>1</v>
@@ -588,7 +588,7 @@
         <v>0.0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -608,15 +608,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -710,16 +710,16 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +741,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>

</xml_diff>